<commit_message>
update sheet copy method
</commit_message>
<xml_diff>
--- a/resources/templates/ebom.xlsx
+++ b/resources/templates/ebom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC66CE4B-A454-4859-87E3-2654713DB754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EE6FE8-8ADE-4521-A588-0902CC264A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -250,7 +250,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,12 +308,6 @@
     </font>
     <font>
       <b/>
-      <sz val="8"/>
-      <color theme="0" tint="-4.9989318521683403E-2"/>
-      <name val="Cascadia Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color theme="0" tint="-4.9989318521683403E-2"/>
       <name val="Cascadia Mono"/>
@@ -397,7 +391,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -433,14 +427,11 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -790,7 +781,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.25"/>
@@ -811,39 +802,39 @@
     <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
     </row>
-    <row r="2" spans="1:13" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
@@ -1006,7 +997,7 @@
       <c r="G8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="16" t="s">
         <v>29</v>
       </c>
       <c r="I8" s="16"/>
@@ -1016,9 +1007,10 @@
       <c r="M8" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:M2"/>
+    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix - Export 格式 merged cell
</commit_message>
<xml_diff>
--- a/resources/templates/ebom.xlsx
+++ b/resources/templates/ebom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC66CE4B-A454-4859-87E3-2654713DB754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBD99AC-5E22-4647-B8F4-36BB63A5888D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -250,7 +250,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,12 +308,6 @@
     </font>
     <font>
       <b/>
-      <sz val="8"/>
-      <color theme="0" tint="-4.9989318521683403E-2"/>
-      <name val="Cascadia Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color theme="0" tint="-4.9989318521683403E-2"/>
       <name val="Cascadia Mono"/>
@@ -397,7 +391,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -433,14 +427,11 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -790,7 +781,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.25"/>
@@ -812,38 +803,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
@@ -1006,7 +997,7 @@
       <c r="G8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="16" t="s">
         <v>29</v>
       </c>
       <c r="I8" s="16"/>
@@ -1016,9 +1007,10 @@
       <c r="M8" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:M2"/>
+    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix side bar resize
</commit_message>
<xml_diff>
--- a/resources/templates/ebom.xlsx
+++ b/resources/templates/ebom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBD99AC-5E22-4647-B8F4-36BB63A5888D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A3E922-A3D6-4DBF-9695-487C7423D35C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -781,7 +781,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E7" sqref="E7:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.25"/>

</xml_diff>